<commit_message>
Data prep and cleaning
Started the data cleaning and preperation part of the project
</commit_message>
<xml_diff>
--- a/NLP_what_defines_a_data_scientist.xlsx
+++ b/NLP_what_defines_a_data_scientist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Louis\Documents\Data_science_stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Louis\Documents\Data_science_stuff\NLP_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6EC860ED-AC84-4C90-A046-0FE0CD812848}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B573FC-6D49-4A69-8777-855B829A7AF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="315" windowWidth="23625" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7920" yWindow="15" windowWidth="20835" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,15 +29,114 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Qualifications</t>
+  </si>
+  <si>
+    <t>Responsibilities</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Mid-Senior level</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Data Scientist</t>
+  </si>
+  <si>
+    <t>Scientific Research &amp; Development</t>
+  </si>
+  <si>
+    <t>Southampton</t>
+  </si>
+  <si>
+    <t>Linkedin</t>
+  </si>
+  <si>
+    <t>Educated to bachelor’s degree (or higher) in a numerate discipline, such as mathematics, statistics, computer science, data science, or a related field with a significant statistics bias
+Experience in programming in Python and the ability to write readable, efficient code
+Experience of C or C++ or Java, Perl, Matlab, R is also beneficial
+Experience of developing, testing of machine-learning models
+Demonstrate experience of supervised learning, unsupervised learning is desirable
+Good applied statistics skills, such as distributions, statistical testing, regression, etc.
+Solid understanding of databases &amp; SQL
+Experience in data visualization tools - experience of PowerBi or Tableau beneficial
+Clear communicator - able to concisely communicate complex issues &amp; techniques deployed to both technical and non-technical audiences in an effective manner both verbally and in writing
+Good business acumen</t>
+  </si>
+  <si>
+    <t>Derive, new valuable actionable insights from data and communicate effectively to stakeholders and decision makers
+Solve problems in fundamental scientific research using data-driven insights
+Develop proprietary algorithms, using data analytical methodologies
+Develop studies to create the necessary training data, as and when required
+Collect, organize and visualize large sets of structured and unstructured data
+Analise, learn and interpret large amounts of data to discover solutions and opportunities to improving all aspects of our products and digital ecosystem
+Establish data visualisation toolkit to enable clear communication of techniques used and insights yielded
+Work with the wider team implement these findings into future analytical research tools, and consumer products
+Participate in relevant cross R&amp;D forums related to data science and big data</t>
+  </si>
+  <si>
+    <t>Entry level</t>
+  </si>
+  <si>
+    <t>Information Technology  Analyst  Science</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Statistical modelling and skills in data analytics
+Strong attention to detail and ability to retain information
+Adept using at least one of the common analytical programming languages, eg. R, Python, C++
+BSc in Maths, Statistics, Computer Science, Engineering, or other Quantitative disciplines</t>
+  </si>
+  <si>
+    <t>Interpret data, analyse results using statistical techniques, and provide reports
+Acquire data from multiple data sources, filtering, cleaning and wrapping
+Identify, analyse, and interpret trends or patterns in complex data sets
+Work with senior colleagues to prioritise business and information needs
+Locate and define new process improvement opportunities
+Operate with Python as your primary language</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -60,8 +159,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,14 +491,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="7" width="90.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="90.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completed NLP for responsibilities too
</commit_message>
<xml_diff>
--- a/NLP_what_defines_a_data_scientist.xlsx
+++ b/NLP_what_defines_a_data_scientist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Louis\Documents\Data_science_stuff\NLP_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5AC57B9-4037-4EDA-8561-5EAE17523D43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ACE909D-204C-4190-8C55-2ED2B5464990}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="270" yWindow="90" windowWidth="16080" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="66">
   <si>
     <t>Role</t>
   </si>
@@ -332,6 +332,47 @@
     <t>To be considered for this role, you will understand statistical and predictive modelling concepts, machine-learning approaches, clustering and classification techniques, and recommendation and optimization algorithms.
 You will have a passion for analysing large, complex, multi-dimensional datasets with a variety of tools. You have an awareness and some experience of statistical analysis environments such as R, MATLAB, SPSS or SAS. You have experience with BI tools such as Tableau and MicroStrategy. You’re as comfortable with relational databases as you are with data mining frameworks. You are also familiar with SQL, Python, Java and C/C++.
 This is an excellent opportunity to work for with a dynamic and forward thinking organisation.</t>
+  </si>
+  <si>
+    <t>Data Scientists are split into two paths, depending on your experience and career aspirations: Commercial where you will be working with clients to tailor the predictive machine to their specific needs; and Research where you will work purely in-house to develop new models.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Strong academic record – PhD or Master’s in ML/Maths/Stats etc. – from a leading university
+Creative mind and ability to come up with new ideas to solve complex problems
+Experience publishing journals is also highly sought-after
+Excellent written and verbal communication skills</t>
+  </si>
+  <si>
+    <t>Oxford Knight Limited</t>
+  </si>
+  <si>
+    <t>Davies group</t>
+  </si>
+  <si>
+    <t>You will recommend statistical/machine learning tools and technologies to prototype new concepts.
+You must be able to carry out statistical analysis including data modelling &amp; hypothesis testing.
+You must be able to retrieve and collect open and closed data sources, including data processing, cleansing and verification.
+Where applicable, you will work with developers to integrate specialist third party applications.
+You will be the subject matter expert for machine learning techniques, aiding the development of solutions for real world problems.
+You will be a mentor and coach to less experienced colleagues.
+You will work closely with the Head of Infrastructure and Programmes to ensure IT objectives are achieved</t>
+  </si>
+  <si>
+    <t>We work to an Agile Scrum framework and are currently undergoing a transition to DevOps so it would be great if you have experience in these areas.
+You will be an expert in machine learning &amp; data classification and will also have demonstrable experience in Python. Any legal/case management experience would also be a bonus.
+Teamwork – You will contribute actively to an environment in which colleagues work cooperatively with each other.
+Agile – Experience of Agile Scrum methodology is an advantage.
+Concern for Excellence – You must understand the Principles of Excellence at Keoghs and how these are applied to the way Keoghs runs its business.
+You must understand and adhere to Keoghs Shared Values.
+You will be self-motivated with a strong work ethic who can work without supervision.
+You must show a highly committed attitude.
+You must have good analytical skills, methodical, accurate and show great attention to detail.
+You will be able to communicate in clear and concise manner both written and verbal.
+You must be flexible/adaptable to change.</t>
+  </si>
+  <si>
+    <t>Manchester</t>
   </si>
 </sst>
 </file>
@@ -714,10 +755,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,6 +1137,58 @@
         <v>57</v>
       </c>
     </row>
+    <row r="15" spans="1:9" ht="120.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15">
+        <v>68</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="240.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16">
+        <v>43</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>